<commit_message>
fixed HDR bug - faulty filterbam file association with multiple tumor samples for one normal
</commit_message>
<xml_diff>
--- a/info/filter_settings.xlsx
+++ b/info/filter_settings.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinscience/Dropbox/Icke/Work/somVar/FDAH/info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/Dropbox/Icke/Work/somVar/FDAH/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356A2F56-14C1-6546-969B-2E207C8065D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216A1DDC-F4F7-9040-BF3D-A1B998EF59CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="700" windowWidth="28040" windowHeight="16540" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22760" windowHeight="19640" activeTab="2" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
   </bookViews>
   <sheets>
-    <sheet name="AML" sheetId="1" r:id="rId1"/>
+    <sheet name="AMLMono7" sheetId="1" r:id="rId1"/>
+    <sheet name="NHL" sheetId="2" r:id="rId2"/>
+    <sheet name="AMLValidation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>filter1</t>
   </si>
@@ -70,16 +72,89 @@
   </si>
   <si>
     <t>EBscore</t>
+  </si>
+  <si>
+    <t>minimal number of reads supporting Alt</t>
+  </si>
+  <si>
+    <t>read coverage in tumor</t>
+  </si>
+  <si>
+    <t>significance relative to Panel of Normal</t>
+  </si>
+  <si>
+    <t>how many Alt calls in the entire Panel of Normals</t>
+  </si>
+  <si>
+    <t>difference of strand bias between Alt reads and Ref reads</t>
+  </si>
+  <si>
+    <t>tumor VAF</t>
+  </si>
+  <si>
+    <t>normal VAF</t>
+  </si>
+  <si>
+    <t>Clinical Score computed from all Clinical data</t>
+  </si>
+  <si>
+    <t>HDRcount</t>
+  </si>
+  <si>
+    <t>number of significant HDRlanes around mutation</t>
+  </si>
+  <si>
+    <t>how should the VAF be for Mutations in Candidate Genes</t>
+  </si>
+  <si>
+    <t>TVAF4Cand</t>
+  </si>
+  <si>
+    <t>strandPolarity</t>
+  </si>
+  <si>
+    <t>maximum fraction of reads in one direction</t>
+  </si>
+  <si>
+    <t>notes ext</t>
+  </si>
+  <si>
+    <t>str10' filter in VARSCAN uses 10%</t>
+  </si>
+  <si>
+    <t>VAFRatio</t>
+  </si>
+  <si>
+    <t>maximum TVAF/NVAF</t>
+  </si>
+  <si>
+    <t>sets minimum reduction in NVAF relative to TVAF</t>
+  </si>
+  <si>
+    <t>PopFreq</t>
+  </si>
+  <si>
+    <t>VAFSim</t>
+  </si>
+  <si>
+    <t>exclude similarVAF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,8 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,19 +498,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D898A62A-F689-E746-ADB1-1D4B92D37F0D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -453,16 +531,31 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -484,14 +577,15 @@
       <c r="G2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.02</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -514,16 +608,31 @@
         <v>40</v>
       </c>
       <c r="H3">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="I3">
+        <v>0.04</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
         <v>0.4</v>
       </c>
-      <c r="J3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -546,16 +655,31 @@
         <v>30</v>
       </c>
       <c r="H4">
+        <v>0.95</v>
+      </c>
+      <c r="I4">
+        <v>0.04</v>
+      </c>
+      <c r="J4">
+        <v>0.03</v>
+      </c>
+      <c r="K4">
+        <v>0.35</v>
+      </c>
+      <c r="L4">
+        <v>0.9</v>
+      </c>
+      <c r="M4">
+        <v>400</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" s="2">
         <v>0.02</v>
       </c>
-      <c r="I4">
-        <v>0.35</v>
-      </c>
-      <c r="J4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -578,16 +702,29 @@
         <v>20</v>
       </c>
       <c r="H5">
+        <v>0.9</v>
+      </c>
+      <c r="I5">
+        <v>0.05</v>
+      </c>
+      <c r="J5">
         <v>0.03</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.25</v>
       </c>
-      <c r="J5">
+      <c r="L5">
+        <v>0.8</v>
+      </c>
+      <c r="M5">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -618,10 +755,730 @@
       <c r="J6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B377FCD4-B7F7-6041-9782-9B6AE8A87EDF}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1E-3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="K2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.04</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>0.95</v>
+      </c>
+      <c r="I4">
+        <v>0.04</v>
+      </c>
+      <c r="J4">
+        <v>0.03</v>
+      </c>
+      <c r="K4">
+        <v>0.15</v>
+      </c>
+      <c r="L4">
+        <v>0.9</v>
+      </c>
+      <c r="M4">
+        <v>400</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>0.9</v>
+      </c>
+      <c r="I5">
+        <v>0.05</v>
+      </c>
+      <c r="J5">
+        <v>0.03</v>
+      </c>
+      <c r="K5">
+        <v>0.1</v>
+      </c>
+      <c r="L5">
+        <v>0.8</v>
+      </c>
+      <c r="M5">
+        <v>2000</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452FF9F4-C447-3948-8FA8-B5FA47A4265F}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1E-3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="K2">
+        <v>0.3</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.02</v>
+      </c>
+      <c r="J3">
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <v>0.9</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>200</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1E-4</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>0.95</v>
+      </c>
+      <c r="I4">
+        <v>0.03</v>
+      </c>
+      <c r="J4">
+        <v>0.03</v>
+      </c>
+      <c r="K4">
+        <v>0.8</v>
+      </c>
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+      <c r="M4">
+        <v>500</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>0.9</v>
+      </c>
+      <c r="I5">
+        <v>0.05</v>
+      </c>
+      <c r="J5">
+        <v>0.03</v>
+      </c>
+      <c r="K5">
+        <v>0.7</v>
+      </c>
+      <c r="L5">
+        <v>0.2</v>
+      </c>
+      <c r="M5">
+        <v>2000</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed Primer3 AmpliconSize bug
</commit_message>
<xml_diff>
--- a/info/filter_settings.xlsx
+++ b/info/filter_settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/Dropbox/Icke/Work/somVar/FDAH/info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/mount/snakes/develop/somVarWES/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216A1DDC-F4F7-9040-BF3D-A1B998EF59CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D1BF74-90B8-044F-A729-A84E8C1C5D52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22760" windowHeight="19640" activeTab="2" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
+    <workbookView xWindow="17580" yWindow="-22920" windowWidth="22760" windowHeight="19640" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
   </bookViews>
   <sheets>
     <sheet name="AMLMono7" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D898A62A-F689-E746-ADB1-1D4B92D37F0D}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,18 +572,17 @@
         <v>1E-3</v>
       </c>
       <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0.02</v>
       </c>
       <c r="K2">
-        <v>0.3</v>
-      </c>
-      <c r="O2" s="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -722,7 +721,9 @@
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="2">
+        <v>1E-4</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1156,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452FF9F4-C447-3948-8FA8-B5FA47A4265F}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed filter issues + started SLURM implementation
</commit_message>
<xml_diff>
--- a/info/filter_settings.xlsx
+++ b/info/filter_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/mount/snakes/develop/somVarWES/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D1BF74-90B8-044F-A729-A84E8C1C5D52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3409C3C4-2569-EF43-BA04-FBD9DCF9D7B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="-22920" windowWidth="22760" windowHeight="19640" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
+    <workbookView xWindow="-7180" yWindow="-21020" windowWidth="23300" windowHeight="19300" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
   </bookViews>
   <sheets>
     <sheet name="AMLMono7" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
   <si>
     <t>filter1</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>str10' filter in VARSCAN uses 10%</t>
-  </si>
-  <si>
-    <t>VAFRatio</t>
-  </si>
-  <si>
-    <t>maximum TVAF/NVAF</t>
   </si>
   <si>
     <t>sets minimum reduction in NVAF relative to TVAF</t>
@@ -501,7 +495,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +537,7 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -552,7 +546,7 @@
         <v>23</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -619,7 +613,7 @@
         <v>0.4</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>100</v>
@@ -666,7 +660,7 @@
         <v>0.35</v>
       </c>
       <c r="L4">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="M4">
         <v>400</v>
@@ -713,7 +707,7 @@
         <v>0.25</v>
       </c>
       <c r="L5">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -801,7 +795,7 @@
         <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
@@ -818,7 +812,7 @@
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +825,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="L1" sqref="L1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,7 +867,7 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -882,7 +876,7 @@
         <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -913,6 +907,7 @@
       <c r="K2">
         <v>0.3</v>
       </c>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -949,7 +944,7 @@
         <v>0.2</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>100</v>
@@ -957,7 +952,7 @@
       <c r="N3">
         <v>6</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <v>0.08</v>
       </c>
     </row>
@@ -996,7 +991,7 @@
         <v>0.15</v>
       </c>
       <c r="L4">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="M4">
         <v>400</v>
@@ -1004,7 +999,7 @@
       <c r="N4">
         <v>3</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>0.02</v>
       </c>
     </row>
@@ -1043,13 +1038,16 @@
         <v>0.1</v>
       </c>
       <c r="L5">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="M5">
         <v>2000</v>
       </c>
       <c r="N5">
         <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1128,7 +1126,7 @@
         <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
@@ -1145,7 +1143,7 @@
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1158,13 +1156,13 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L8" sqref="L1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
   </cols>
@@ -1201,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -1210,7 +1208,7 @@
         <v>23</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1462,7 +1460,7 @@
         <v>21</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
@@ -1479,7 +1477,7 @@
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved filter output and VAFSIM
</commit_message>
<xml_diff>
--- a/info/filter_settings.xlsx
+++ b/info/filter_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtin/mount/snakes/develop/somVarWES/info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinscience/mount/snakes/develop/somVarWES/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3409C3C4-2569-EF43-BA04-FBD9DCF9D7B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61B9ECE-1729-484C-B70F-CA1BA5C9DFA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7180" yWindow="-21020" windowWidth="23300" windowHeight="19300" xr2:uid="{B2573AEE-7AC4-F745-A872-CAAD802DC491}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>filter1</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>exclude similarVAF</t>
+  </si>
+  <si>
+    <t>sets maximum fraction of  NVAF relative to TVAF</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -574,7 +577,7 @@
       <c r="K2">
         <v>0.9</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>0.1</v>
       </c>
     </row>
@@ -613,7 +616,7 @@
         <v>0.4</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="M3">
         <v>100</v>
@@ -621,7 +624,7 @@
       <c r="N3">
         <v>6</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3">
         <v>0.08</v>
       </c>
     </row>
@@ -660,16 +663,16 @@
         <v>0.35</v>
       </c>
       <c r="L4">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="M4">
         <v>400</v>
       </c>
       <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.02</v>
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -707,7 +710,7 @@
         <v>0.25</v>
       </c>
       <c r="L5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -715,7 +718,7 @@
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5">
         <v>1E-4</v>
       </c>
     </row>
@@ -812,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>